<commit_message>
Checking on microstructure one-hot-encoder
</commit_message>
<xml_diff>
--- a/04_Model_Saved/NN_full_v3_BO_optimal/MultiTaskModel_NiCrCoVFe_KW99_wt_pct_ML_mc_shared_relu.xlsx
+++ b/04_Model_Saved/NN_full_v3_BO_optimal/MultiTaskModel_NiCrCoVFe_KW99_wt_pct_ML_mc_shared_relu.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,20 +466,25 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>microstructure</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>H1_new_pred_KFold_mean</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>H1_new_pred_KFold_std</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>C2_new_pred_KFold_mean</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>C2_new_pred_KFold_std</t>
         </is>
@@ -504,17 +509,22 @@
       <c r="F2" t="n">
         <v>10.27148578895017</v>
       </c>
-      <c r="G2" t="n">
-        <v>233.6294250488281</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H2" t="n">
-        <v>56.06689071655273</v>
+        <v>220.6301574707031</v>
       </c>
       <c r="I2" t="n">
-        <v>474.7901000976562</v>
+        <v>59.1779899597168</v>
       </c>
       <c r="J2" t="n">
-        <v>115.5027694702148</v>
+        <v>499.4284973144531</v>
+      </c>
+      <c r="K2" t="n">
+        <v>96.36595916748047</v>
       </c>
     </row>
     <row r="3">
@@ -536,17 +546,22 @@
       <c r="F3" t="n">
         <v>10.49540628405087</v>
       </c>
-      <c r="G3" t="n">
-        <v>244.2517242431641</v>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H3" t="n">
-        <v>53.85313415527344</v>
+        <v>227.9122467041016</v>
       </c>
       <c r="I3" t="n">
-        <v>497.0472412109375</v>
+        <v>62.01198196411133</v>
       </c>
       <c r="J3" t="n">
-        <v>123.682014465332</v>
+        <v>541.3877563476562</v>
+      </c>
+      <c r="K3" t="n">
+        <v>108.6241073608398</v>
       </c>
     </row>
     <row r="4">
@@ -568,17 +583,22 @@
       <c r="F4" t="n">
         <v>11.11292799977388</v>
       </c>
-      <c r="G4" t="n">
-        <v>255.5135192871094</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H4" t="n">
-        <v>59.15281295776367</v>
+        <v>241.4866180419922</v>
       </c>
       <c r="I4" t="n">
-        <v>520.8933715820312</v>
+        <v>59.25140762329102</v>
       </c>
       <c r="J4" t="n">
-        <v>133.0312652587891</v>
+        <v>564.2969970703125</v>
+      </c>
+      <c r="K4" t="n">
+        <v>122.0126190185547</v>
       </c>
     </row>
     <row r="5">
@@ -600,17 +620,22 @@
       <c r="F5" t="n">
         <v>11.33579528302992</v>
       </c>
-      <c r="G5" t="n">
-        <v>270.7007751464844</v>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H5" t="n">
-        <v>62.98183822631836</v>
+        <v>258.3315124511719</v>
       </c>
       <c r="I5" t="n">
-        <v>539.0090942382812</v>
+        <v>60.15779876708984</v>
       </c>
       <c r="J5" t="n">
-        <v>137.4183349609375</v>
+        <v>586.85498046875</v>
+      </c>
+      <c r="K5" t="n">
+        <v>123.6608963012695</v>
       </c>
     </row>
     <row r="6">
@@ -632,17 +657,22 @@
       <c r="F6" t="n">
         <v>11.53221857575777</v>
       </c>
-      <c r="G6" t="n">
-        <v>279.1702575683594</v>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H6" t="n">
-        <v>72.24607086181641</v>
+        <v>273.2442932128906</v>
       </c>
       <c r="I6" t="n">
-        <v>531.3665161132812</v>
+        <v>70.79751586914062</v>
       </c>
       <c r="J6" t="n">
-        <v>148.1827545166016</v>
+        <v>569.216064453125</v>
+      </c>
+      <c r="K6" t="n">
+        <v>115.4581298828125</v>
       </c>
     </row>
     <row r="7">
@@ -664,17 +694,22 @@
       <c r="F7" t="n">
         <v>11.73836346032553</v>
       </c>
-      <c r="G7" t="n">
-        <v>203.7388000488281</v>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H7" t="n">
-        <v>58.05046081542969</v>
+        <v>189.94580078125</v>
       </c>
       <c r="I7" t="n">
-        <v>395.1377868652344</v>
+        <v>62.2507209777832</v>
       </c>
       <c r="J7" t="n">
-        <v>80.14458465576172</v>
+        <v>408.1087341308594</v>
+      </c>
+      <c r="K7" t="n">
+        <v>84.58387756347656</v>
       </c>
     </row>
     <row r="8">
@@ -696,17 +731,22 @@
       <c r="F8" t="n">
         <v>12.47588443056982</v>
       </c>
-      <c r="G8" t="n">
-        <v>216.1732635498047</v>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H8" t="n">
-        <v>55.38935470581055</v>
+        <v>202.5159759521484</v>
       </c>
       <c r="I8" t="n">
-        <v>428.7518615722656</v>
+        <v>58.26871871948242</v>
       </c>
       <c r="J8" t="n">
-        <v>99.78487396240234</v>
+        <v>449.1215209960938</v>
+      </c>
+      <c r="K8" t="n">
+        <v>83.82854461669922</v>
       </c>
     </row>
     <row r="9">
@@ -728,17 +768,22 @@
       <c r="F9" t="n">
         <v>13.31360035996819</v>
       </c>
-      <c r="G9" t="n">
-        <v>228.1960601806641</v>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H9" t="n">
-        <v>51.11914825439453</v>
+        <v>215.523681640625</v>
       </c>
       <c r="I9" t="n">
-        <v>450.914794921875</v>
+        <v>58.67217254638672</v>
       </c>
       <c r="J9" t="n">
-        <v>106.8655395507812</v>
+        <v>474.5057373046875</v>
+      </c>
+      <c r="K9" t="n">
+        <v>85.06479644775391</v>
       </c>
     </row>
     <row r="10">
@@ -760,17 +805,22 @@
       <c r="F10" t="n">
         <v>14.04586286313179</v>
       </c>
-      <c r="G10" t="n">
-        <v>244.2298431396484</v>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H10" t="n">
-        <v>47.3739128112793</v>
+        <v>223.4780731201172</v>
       </c>
       <c r="I10" t="n">
-        <v>456.7231750488281</v>
+        <v>65.33212280273438</v>
       </c>
       <c r="J10" t="n">
-        <v>113.5271377563477</v>
+        <v>490.3695373535156</v>
+      </c>
+      <c r="K10" t="n">
+        <v>88.62237548828125</v>
       </c>
     </row>
     <row r="11">
@@ -792,17 +842,22 @@
       <c r="F11" t="n">
         <v>14.78596965177877</v>
       </c>
-      <c r="G11" t="n">
-        <v>260.2477111816406</v>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H11" t="n">
-        <v>52.34081268310547</v>
+        <v>236.1459045410156</v>
       </c>
       <c r="I11" t="n">
-        <v>471.1871948242188</v>
+        <v>65.01383972167969</v>
       </c>
       <c r="J11" t="n">
-        <v>121.0184936523438</v>
+        <v>519.798095703125</v>
+      </c>
+      <c r="K11" t="n">
+        <v>96.54000091552734</v>
       </c>
     </row>
     <row r="12">
@@ -824,17 +879,22 @@
       <c r="F12" t="n">
         <v>14.60750023008277</v>
       </c>
-      <c r="G12" t="n">
-        <v>270.4848937988281</v>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H12" t="n">
-        <v>58.20036315917969</v>
+        <v>245.9027099609375</v>
       </c>
       <c r="I12" t="n">
-        <v>472.7792663574219</v>
+        <v>65.56962585449219</v>
       </c>
       <c r="J12" t="n">
-        <v>124.1278610229492</v>
+        <v>515.2958984375</v>
+      </c>
+      <c r="K12" t="n">
+        <v>104.872444152832</v>
       </c>
     </row>
     <row r="13">
@@ -856,17 +916,22 @@
       <c r="F13" t="n">
         <v>13.93632017907879</v>
       </c>
-      <c r="G13" t="n">
-        <v>293.0524597167969</v>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H13" t="n">
-        <v>66.84127044677734</v>
+        <v>271.25390625</v>
       </c>
       <c r="I13" t="n">
-        <v>481.4786071777344</v>
+        <v>72.53400421142578</v>
       </c>
       <c r="J13" t="n">
-        <v>136.6026916503906</v>
+        <v>512.9419555664062</v>
+      </c>
+      <c r="K13" t="n">
+        <v>118.7576293945312</v>
       </c>
     </row>
     <row r="14">
@@ -888,17 +953,22 @@
       <c r="F14" t="n">
         <v>13.2060787967079</v>
       </c>
-      <c r="G14" t="n">
-        <v>165.6684112548828</v>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H14" t="n">
-        <v>71.30052185058594</v>
+        <v>162.797607421875</v>
       </c>
       <c r="I14" t="n">
-        <v>204.6610870361328</v>
+        <v>71.98178863525391</v>
       </c>
       <c r="J14" t="n">
-        <v>73.81336975097656</v>
+        <v>223.3926086425781</v>
+      </c>
+      <c r="K14" t="n">
+        <v>92.37525939941406</v>
       </c>
     </row>
     <row r="15">
@@ -920,17 +990,22 @@
       <c r="F15" t="n">
         <v>14.43724685121477</v>
       </c>
-      <c r="G15" t="n">
-        <v>185.0393218994141</v>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H15" t="n">
-        <v>66.71070098876953</v>
+        <v>174.5071411132812</v>
       </c>
       <c r="I15" t="n">
-        <v>268.706298828125</v>
+        <v>68.25331115722656</v>
       </c>
       <c r="J15" t="n">
-        <v>72.76538848876953</v>
+        <v>289.2753601074219</v>
+      </c>
+      <c r="K15" t="n">
+        <v>93.64822387695312</v>
       </c>
     </row>
     <row r="16">
@@ -952,17 +1027,22 @@
       <c r="F16" t="n">
         <v>15.77509757365795</v>
       </c>
-      <c r="G16" t="n">
-        <v>200.7733917236328</v>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H16" t="n">
-        <v>59.21551895141602</v>
+        <v>187.0930023193359</v>
       </c>
       <c r="I16" t="n">
-        <v>329.3307495117188</v>
+        <v>62.70480346679688</v>
       </c>
       <c r="J16" t="n">
-        <v>66.22640991210938</v>
+        <v>343.223876953125</v>
+      </c>
+      <c r="K16" t="n">
+        <v>90.07003021240234</v>
       </c>
     </row>
     <row r="17">
@@ -984,17 +1064,22 @@
       <c r="F17" t="n">
         <v>17.01643502058164</v>
       </c>
-      <c r="G17" t="n">
-        <v>218.9375457763672</v>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H17" t="n">
-        <v>53.22798919677734</v>
+        <v>202.7883911132812</v>
       </c>
       <c r="I17" t="n">
-        <v>386.2823486328125</v>
+        <v>63.29397201538086</v>
       </c>
       <c r="J17" t="n">
-        <v>81.4444580078125</v>
+        <v>401.7761535644531</v>
+      </c>
+      <c r="K17" t="n">
+        <v>82.61502838134766</v>
       </c>
     </row>
     <row r="18">
@@ -1016,17 +1101,22 @@
       <c r="F18" t="n">
         <v>17.57324774662381</v>
       </c>
-      <c r="G18" t="n">
-        <v>224.8482818603516</v>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H18" t="n">
-        <v>47.37125778198242</v>
+        <v>210.9923248291016</v>
       </c>
       <c r="I18" t="n">
-        <v>408.8973083496094</v>
+        <v>62.68314743041992</v>
       </c>
       <c r="J18" t="n">
-        <v>89.39891815185547</v>
+        <v>434.2683410644531</v>
+      </c>
+      <c r="K18" t="n">
+        <v>85.14745330810547</v>
       </c>
     </row>
     <row r="19">
@@ -1048,17 +1138,22 @@
       <c r="F19" t="n">
         <v>18.2282289394109</v>
       </c>
-      <c r="G19" t="n">
-        <v>241.7953338623047</v>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H19" t="n">
-        <v>47.15690612792969</v>
+        <v>221.4175262451172</v>
       </c>
       <c r="I19" t="n">
-        <v>427.3316345214844</v>
+        <v>64.07367706298828</v>
       </c>
       <c r="J19" t="n">
-        <v>97.81977844238281</v>
+        <v>457.6764526367188</v>
+      </c>
+      <c r="K19" t="n">
+        <v>86.85099029541016</v>
       </c>
     </row>
     <row r="20">
@@ -1080,17 +1175,22 @@
       <c r="F20" t="n">
         <v>18.05168677518481</v>
       </c>
-      <c r="G20" t="n">
-        <v>259.3960266113281</v>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H20" t="n">
-        <v>44.3876953125</v>
+        <v>227.9962463378906</v>
       </c>
       <c r="I20" t="n">
-        <v>438.2647399902344</v>
+        <v>64.71458435058594</v>
       </c>
       <c r="J20" t="n">
-        <v>111.8029556274414</v>
+        <v>475.9619750976562</v>
+      </c>
+      <c r="K20" t="n">
+        <v>101.4739837646484</v>
       </c>
     </row>
     <row r="21">
@@ -1112,17 +1212,22 @@
       <c r="F21" t="n">
         <v>17.30316829702608</v>
       </c>
-      <c r="G21" t="n">
-        <v>282.7537231445312</v>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H21" t="n">
-        <v>51.17500305175781</v>
+        <v>254.0884399414062</v>
       </c>
       <c r="I21" t="n">
-        <v>449.6344909667969</v>
+        <v>60.8999137878418</v>
       </c>
       <c r="J21" t="n">
-        <v>122.1962585449219</v>
+        <v>472.7930297851562</v>
+      </c>
+      <c r="K21" t="n">
+        <v>109.6866455078125</v>
       </c>
     </row>
     <row r="22">
@@ -1144,17 +1249,22 @@
       <c r="F22" t="n">
         <v>15.87142913305469</v>
       </c>
-      <c r="G22" t="n">
-        <v>333.3799438476562</v>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H22" t="n">
-        <v>80.86070251464844</v>
+        <v>319.4763793945312</v>
       </c>
       <c r="I22" t="n">
-        <v>451.7577514648438</v>
+        <v>93.06650543212891</v>
       </c>
       <c r="J22" t="n">
-        <v>136.0855102539062</v>
+        <v>444.5184326171875</v>
+      </c>
+      <c r="K22" t="n">
+        <v>141.9555511474609</v>
       </c>
     </row>
     <row r="23">
@@ -1176,17 +1286,22 @@
       <c r="F23" t="n">
         <v>16.2842163689804</v>
       </c>
-      <c r="G23" t="n">
-        <v>155.5232238769531</v>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H23" t="n">
-        <v>79.68890380859375</v>
+        <v>153.5684051513672</v>
       </c>
       <c r="I23" t="n">
-        <v>124.7247924804688</v>
+        <v>72.91082000732422</v>
       </c>
       <c r="J23" t="n">
-        <v>76.03273773193359</v>
+        <v>147.1275024414062</v>
+      </c>
+      <c r="K23" t="n">
+        <v>91.37540435791016</v>
       </c>
     </row>
     <row r="24">
@@ -1208,17 +1323,22 @@
       <c r="F24" t="n">
         <v>17.99859633271077</v>
       </c>
-      <c r="G24" t="n">
-        <v>170.3216705322266</v>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H24" t="n">
-        <v>71.50062561035156</v>
+        <v>169.1233825683594</v>
       </c>
       <c r="I24" t="n">
-        <v>173.7071990966797</v>
+        <v>69.53512573242188</v>
       </c>
       <c r="J24" t="n">
-        <v>80.75071716308594</v>
+        <v>202.8737945556641</v>
+      </c>
+      <c r="K24" t="n">
+        <v>94.65643310546875</v>
       </c>
     </row>
     <row r="25">
@@ -1240,17 +1360,22 @@
       <c r="F25" t="n">
         <v>19.53665474474453</v>
       </c>
-      <c r="G25" t="n">
-        <v>184.9808044433594</v>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H25" t="n">
-        <v>66.21535491943359</v>
+        <v>175.9492034912109</v>
       </c>
       <c r="I25" t="n">
-        <v>212.3995056152344</v>
+        <v>68.94805908203125</v>
       </c>
       <c r="J25" t="n">
-        <v>83.11348724365234</v>
+        <v>250.8156585693359</v>
+      </c>
+      <c r="K25" t="n">
+        <v>91.49556732177734</v>
       </c>
     </row>
     <row r="26">
@@ -1272,17 +1397,22 @@
       <c r="F26" t="n">
         <v>21.18080958029204</v>
       </c>
-      <c r="G26" t="n">
-        <v>202.8692779541016</v>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H26" t="n">
-        <v>62.60544204711914</v>
+        <v>187.2120666503906</v>
       </c>
       <c r="I26" t="n">
-        <v>269.8469848632812</v>
+        <v>70.68913269042969</v>
       </c>
       <c r="J26" t="n">
-        <v>79.40776824951172</v>
+        <v>297.5531005859375</v>
+      </c>
+      <c r="K26" t="n">
+        <v>95.22386169433594</v>
       </c>
     </row>
     <row r="27">
@@ -1304,17 +1434,22 @@
       <c r="F27" t="n">
         <v>22.36133238808863</v>
       </c>
-      <c r="G27" t="n">
-        <v>217.7067108154297</v>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H27" t="n">
-        <v>53.45538711547852</v>
+        <v>200.7974090576172</v>
       </c>
       <c r="I27" t="n">
-        <v>347.4378051757812</v>
+        <v>67.31533813476562</v>
       </c>
       <c r="J27" t="n">
-        <v>67.08443450927734</v>
+        <v>349.1663513183594</v>
+      </c>
+      <c r="K27" t="n">
+        <v>94.59308624267578</v>
       </c>
     </row>
     <row r="28">
@@ -1336,17 +1471,22 @@
       <c r="F28" t="n">
         <v>22.25528267810615</v>
       </c>
-      <c r="G28" t="n">
-        <v>228.7339630126953</v>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H28" t="n">
-        <v>46.41782379150391</v>
+        <v>208.9148712158203</v>
       </c>
       <c r="I28" t="n">
-        <v>382.0462341308594</v>
+        <v>64.68802642822266</v>
       </c>
       <c r="J28" t="n">
-        <v>79.33078765869141</v>
+        <v>393.2320861816406</v>
+      </c>
+      <c r="K28" t="n">
+        <v>96.00433349609375</v>
       </c>
     </row>
     <row r="29">
@@ -1368,17 +1508,22 @@
       <c r="F29" t="n">
         <v>22.11853696692908</v>
       </c>
-      <c r="G29" t="n">
-        <v>246.0581512451172</v>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H29" t="n">
-        <v>42.12464904785156</v>
+        <v>220.1725769042969</v>
       </c>
       <c r="I29" t="n">
-        <v>406.4382019042969</v>
+        <v>64.24864959716797</v>
       </c>
       <c r="J29" t="n">
-        <v>104.8904876708984</v>
+        <v>423.4157104492188</v>
+      </c>
+      <c r="K29" t="n">
+        <v>99.51705169677734</v>
       </c>
     </row>
     <row r="30">
@@ -1400,17 +1545,22 @@
       <c r="F30" t="n">
         <v>21.13587239531939</v>
       </c>
-      <c r="G30" t="n">
-        <v>280.1286926269531</v>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H30" t="n">
-        <v>49.8740119934082</v>
+        <v>251.4181518554688</v>
       </c>
       <c r="I30" t="n">
-        <v>436.9262084960938</v>
+        <v>58.21946334838867</v>
       </c>
       <c r="J30" t="n">
-        <v>131.1773834228516</v>
+        <v>438.8623046875</v>
+      </c>
+      <c r="K30" t="n">
+        <v>114.4740219116211</v>
       </c>
     </row>
     <row r="31">
@@ -1432,17 +1582,22 @@
       <c r="F31" t="n">
         <v>19.80061812897557</v>
       </c>
-      <c r="G31" t="n">
-        <v>323.7873229980469</v>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H31" t="n">
-        <v>74.18986511230469</v>
+        <v>309.0698852539062</v>
       </c>
       <c r="I31" t="n">
-        <v>423.3605041503906</v>
+        <v>73.43027496337891</v>
       </c>
       <c r="J31" t="n">
-        <v>130.0711059570312</v>
+        <v>416.2488403320312</v>
+      </c>
+      <c r="K31" t="n">
+        <v>134.5019989013672</v>
       </c>
     </row>
     <row r="32">
@@ -1464,17 +1619,22 @@
       <c r="F32" t="n">
         <v>20.55168297688286</v>
       </c>
-      <c r="G32" t="n">
-        <v>147.7636108398438</v>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H32" t="n">
-        <v>79.72635650634766</v>
+        <v>151.8853302001953</v>
       </c>
       <c r="I32" t="n">
-        <v>72.56040954589844</v>
+        <v>72.87050628662109</v>
       </c>
       <c r="J32" t="n">
-        <v>72.20065307617188</v>
+        <v>97.30466461181641</v>
+      </c>
+      <c r="K32" t="n">
+        <v>84.21965789794922</v>
       </c>
     </row>
     <row r="33">
@@ -1496,17 +1656,22 @@
       <c r="F33" t="n">
         <v>22.96934284445093</v>
       </c>
-      <c r="G33" t="n">
-        <v>163.3180694580078</v>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H33" t="n">
-        <v>75.41971588134766</v>
+        <v>166.9799957275391</v>
       </c>
       <c r="I33" t="n">
-        <v>104.8023223876953</v>
+        <v>72.73524475097656</v>
       </c>
       <c r="J33" t="n">
-        <v>79.67881774902344</v>
+        <v>137.4281005859375</v>
+      </c>
+      <c r="K33" t="n">
+        <v>96.19129943847656</v>
       </c>
     </row>
     <row r="34">
@@ -1528,17 +1693,22 @@
       <c r="F34" t="n">
         <v>24.40915250803127</v>
       </c>
-      <c r="G34" t="n">
-        <v>180.3034057617188</v>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H34" t="n">
-        <v>67.92824554443359</v>
+        <v>171.1685180664062</v>
       </c>
       <c r="I34" t="n">
-        <v>138.4739379882812</v>
+        <v>74.58148193359375</v>
       </c>
       <c r="J34" t="n">
-        <v>88.04986572265625</v>
+        <v>181.2907867431641</v>
+      </c>
+      <c r="K34" t="n">
+        <v>96.62155151367188</v>
       </c>
     </row>
     <row r="35">
@@ -1560,17 +1730,22 @@
       <c r="F35" t="n">
         <v>26.0811880993595</v>
       </c>
-      <c r="G35" t="n">
-        <v>195.4456939697266</v>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H35" t="n">
-        <v>65.15206146240234</v>
+        <v>181.6549224853516</v>
       </c>
       <c r="I35" t="n">
-        <v>177.3384246826172</v>
+        <v>76.93732452392578</v>
       </c>
       <c r="J35" t="n">
-        <v>91.49510955810547</v>
+        <v>228.3018188476562</v>
+      </c>
+      <c r="K35" t="n">
+        <v>93.11283111572266</v>
       </c>
     </row>
     <row r="36">
@@ -1592,17 +1767,22 @@
       <c r="F36" t="n">
         <v>26.87614780904968</v>
       </c>
-      <c r="G36" t="n">
-        <v>209.6187286376953</v>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H36" t="n">
-        <v>58.06641006469727</v>
+        <v>190.5556030273438</v>
       </c>
       <c r="I36" t="n">
-        <v>239.7773742675781</v>
+        <v>74.77680969238281</v>
       </c>
       <c r="J36" t="n">
-        <v>92.90663146972656</v>
+        <v>274.11328125</v>
+      </c>
+      <c r="K36" t="n">
+        <v>96.08942413330078</v>
       </c>
     </row>
     <row r="37">
@@ -1624,17 +1804,22 @@
       <c r="F37" t="n">
         <v>27.16629873490772</v>
       </c>
-      <c r="G37" t="n">
-        <v>217.6919708251953</v>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H37" t="n">
-        <v>54.0883674621582</v>
+        <v>198.4981384277344</v>
       </c>
       <c r="I37" t="n">
-        <v>290.6998291015625</v>
+        <v>70.83977508544922</v>
       </c>
       <c r="J37" t="n">
-        <v>102.8463439941406</v>
+        <v>309.5693359375</v>
+      </c>
+      <c r="K37" t="n">
+        <v>96.20043182373047</v>
       </c>
     </row>
     <row r="38">
@@ -1656,17 +1841,22 @@
       <c r="F38" t="n">
         <v>27.25598473560972</v>
       </c>
-      <c r="G38" t="n">
-        <v>236.4817504882812</v>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H38" t="n">
-        <v>44.10939025878906</v>
+        <v>212.4986877441406</v>
       </c>
       <c r="I38" t="n">
-        <v>349.026611328125</v>
+        <v>68.62165069580078</v>
       </c>
       <c r="J38" t="n">
-        <v>125.7461395263672</v>
+        <v>372.7648010253906</v>
+      </c>
+      <c r="K38" t="n">
+        <v>101.6739883422852</v>
       </c>
     </row>
     <row r="39">
@@ -1688,17 +1878,22 @@
       <c r="F39" t="n">
         <v>26.04628332899345</v>
       </c>
-      <c r="G39" t="n">
-        <v>268.6336669921875</v>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H39" t="n">
-        <v>46.66052627563477</v>
+        <v>239.8994750976562</v>
       </c>
       <c r="I39" t="n">
-        <v>378.0382080078125</v>
+        <v>61.28727340698242</v>
       </c>
       <c r="J39" t="n">
-        <v>144.3114318847656</v>
+        <v>402.5025024414062</v>
+      </c>
+      <c r="K39" t="n">
+        <v>119.8203353881836</v>
       </c>
     </row>
     <row r="40">
@@ -1720,17 +1915,22 @@
       <c r="F40" t="n">
         <v>23.96978635149335</v>
       </c>
-      <c r="G40" t="n">
-        <v>321.4528503417969</v>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H40" t="n">
-        <v>70.31336975097656</v>
+        <v>305.8853759765625</v>
       </c>
       <c r="I40" t="n">
-        <v>405.2142639160156</v>
+        <v>65.55757141113281</v>
       </c>
       <c r="J40" t="n">
-        <v>134.6981506347656</v>
+        <v>399.8500366210938</v>
+      </c>
+      <c r="K40" t="n">
+        <v>140.1062927246094</v>
       </c>
     </row>
     <row r="41">
@@ -1752,17 +1952,22 @@
       <c r="F41" t="n">
         <v>25.6116837653232</v>
       </c>
-      <c r="G41" t="n">
-        <v>148.2709655761719</v>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H41" t="n">
-        <v>78.57459259033203</v>
+        <v>154.3899536132812</v>
       </c>
       <c r="I41" t="n">
-        <v>33.02262496948242</v>
+        <v>70.94721221923828</v>
       </c>
       <c r="J41" t="n">
-        <v>67.29244232177734</v>
+        <v>68.55633544921875</v>
+      </c>
+      <c r="K41" t="n">
+        <v>81.18212890625</v>
       </c>
     </row>
     <row r="42">
@@ -1784,17 +1989,22 @@
       <c r="F42" t="n">
         <v>28.41067839248494</v>
       </c>
-      <c r="G42" t="n">
-        <v>164.4941864013672</v>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H42" t="n">
-        <v>73.79880523681641</v>
+        <v>164.8587493896484</v>
       </c>
       <c r="I42" t="n">
-        <v>54.3885498046875</v>
+        <v>70.36624145507812</v>
       </c>
       <c r="J42" t="n">
-        <v>72.50645446777344</v>
+        <v>95.14850616455078</v>
+      </c>
+      <c r="K42" t="n">
+        <v>84.79467010498047</v>
       </c>
     </row>
     <row r="43">
@@ -1816,17 +2026,22 @@
       <c r="F43" t="n">
         <v>30.68040031937237</v>
       </c>
-      <c r="G43" t="n">
-        <v>175.7901306152344</v>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H43" t="n">
-        <v>72.93081665039062</v>
+        <v>173.4541473388672</v>
       </c>
       <c r="I43" t="n">
-        <v>76.80331420898438</v>
+        <v>70.18972015380859</v>
       </c>
       <c r="J43" t="n">
-        <v>84.49900054931641</v>
+        <v>129.0738067626953</v>
+      </c>
+      <c r="K43" t="n">
+        <v>90.66093444824219</v>
       </c>
     </row>
     <row r="44">
@@ -1848,17 +2063,22 @@
       <c r="F44" t="n">
         <v>32.34762367758118</v>
       </c>
-      <c r="G44" t="n">
-        <v>192.7582855224609</v>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H44" t="n">
-        <v>66.09413909912109</v>
+        <v>180.1747131347656</v>
       </c>
       <c r="I44" t="n">
-        <v>113.9067077636719</v>
+        <v>73.336181640625</v>
       </c>
       <c r="J44" t="n">
-        <v>97.32958221435547</v>
+        <v>170.5933532714844</v>
+      </c>
+      <c r="K44" t="n">
+        <v>94.78709411621094</v>
       </c>
     </row>
     <row r="45">
@@ -1880,17 +2100,22 @@
       <c r="F45" t="n">
         <v>33.26712421235609</v>
       </c>
-      <c r="G45" t="n">
-        <v>201.1362152099609</v>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H45" t="n">
-        <v>63.83920669555664</v>
+        <v>186.489013671875</v>
       </c>
       <c r="I45" t="n">
-        <v>153.2872619628906</v>
+        <v>82.34949493408203</v>
       </c>
       <c r="J45" t="n">
-        <v>108.8576583862305</v>
+        <v>221.3418273925781</v>
+      </c>
+      <c r="K45" t="n">
+        <v>94.54922485351562</v>
       </c>
     </row>
     <row r="46">
@@ -1912,17 +2137,22 @@
       <c r="F46" t="n">
         <v>33.39925272231932</v>
       </c>
-      <c r="G46" t="n">
-        <v>211.7053070068359</v>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H46" t="n">
-        <v>59.07770156860352</v>
+        <v>196.175048828125</v>
       </c>
       <c r="I46" t="n">
-        <v>233.3243560791016</v>
+        <v>75.77425384521484</v>
       </c>
       <c r="J46" t="n">
-        <v>121.9792404174805</v>
+        <v>276.6124572753906</v>
+      </c>
+      <c r="K46" t="n">
+        <v>103.0248413085938</v>
       </c>
     </row>
     <row r="47">
@@ -1944,17 +2174,22 @@
       <c r="F47" t="n">
         <v>32.83385481517335</v>
       </c>
-      <c r="G47" t="n">
-        <v>223.3578948974609</v>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H47" t="n">
-        <v>51.36756896972656</v>
+        <v>203.1386260986328</v>
       </c>
       <c r="I47" t="n">
-        <v>291.8075866699219</v>
+        <v>69.70423889160156</v>
       </c>
       <c r="J47" t="n">
-        <v>139.3309936523438</v>
+        <v>322.8243103027344</v>
+      </c>
+      <c r="K47" t="n">
+        <v>102.4667129516602</v>
       </c>
     </row>
     <row r="48">
@@ -1976,17 +2211,22 @@
       <c r="F48" t="n">
         <v>31.22587875804939</v>
       </c>
-      <c r="G48" t="n">
-        <v>268.0730285644531</v>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H48" t="n">
-        <v>45.04883193969727</v>
+        <v>242.2288055419922</v>
       </c>
       <c r="I48" t="n">
-        <v>341.9872131347656</v>
+        <v>61.90705108642578</v>
       </c>
       <c r="J48" t="n">
-        <v>156.5239868164062</v>
+        <v>378.8021850585938</v>
+      </c>
+      <c r="K48" t="n">
+        <v>126.1707611083984</v>
       </c>
     </row>
     <row r="49">
@@ -2008,17 +2248,22 @@
       <c r="F49" t="n">
         <v>28.00050845971687</v>
       </c>
-      <c r="G49" t="n">
-        <v>316.072509765625</v>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H49" t="n">
-        <v>68.03215789794922</v>
+        <v>303.1158447265625</v>
       </c>
       <c r="I49" t="n">
-        <v>385.5296936035156</v>
+        <v>65.40548706054688</v>
       </c>
       <c r="J49" t="n">
-        <v>140.4807434082031</v>
+        <v>388.8443603515625</v>
+      </c>
+      <c r="K49" t="n">
+        <v>155.4431304931641</v>
       </c>
     </row>
     <row r="50">
@@ -2040,17 +2285,22 @@
       <c r="F50" t="n">
         <v>32.75859992753161</v>
       </c>
-      <c r="G50" t="n">
-        <v>157.1856231689453</v>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H50" t="n">
-        <v>79.20433807373047</v>
+        <v>159.0690765380859</v>
       </c>
       <c r="I50" t="n">
-        <v>6.909585952758789</v>
+        <v>68.55178070068359</v>
       </c>
       <c r="J50" t="n">
-        <v>68.32032775878906</v>
+        <v>47.4061164855957</v>
+      </c>
+      <c r="K50" t="n">
+        <v>80.5411376953125</v>
       </c>
     </row>
     <row r="51">
@@ -2072,17 +2322,22 @@
       <c r="F51" t="n">
         <v>35.60454595063857</v>
       </c>
-      <c r="G51" t="n">
-        <v>169.4864501953125</v>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H51" t="n">
-        <v>71.66303253173828</v>
+        <v>168.8802795410156</v>
       </c>
       <c r="I51" t="n">
-        <v>17.51554298400879</v>
+        <v>68.2633056640625</v>
       </c>
       <c r="J51" t="n">
-        <v>81.92855072021484</v>
+        <v>63.6456298828125</v>
+      </c>
+      <c r="K51" t="n">
+        <v>79.08767700195312</v>
       </c>
     </row>
     <row r="52">
@@ -2104,17 +2359,22 @@
       <c r="F52" t="n">
         <v>38.13811789539464</v>
       </c>
-      <c r="G52" t="n">
-        <v>182.4219818115234</v>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H52" t="n">
-        <v>69.54685211181641</v>
+        <v>179.1922302246094</v>
       </c>
       <c r="I52" t="n">
-        <v>25.40829658508301</v>
+        <v>71.98125457763672</v>
       </c>
       <c r="J52" t="n">
-        <v>82.61286163330078</v>
+        <v>80.45231628417969</v>
+      </c>
+      <c r="K52" t="n">
+        <v>88.21706390380859</v>
       </c>
     </row>
     <row r="53">
@@ -2136,17 +2396,22 @@
       <c r="F53" t="n">
         <v>39.1380055059179</v>
       </c>
-      <c r="G53" t="n">
-        <v>194.3167572021484</v>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H53" t="n">
-        <v>65.07696533203125</v>
+        <v>185.4116668701172</v>
       </c>
       <c r="I53" t="n">
-        <v>52.25473022460938</v>
+        <v>73.82817840576172</v>
       </c>
       <c r="J53" t="n">
-        <v>91.78582000732422</v>
+        <v>114.206428527832</v>
+      </c>
+      <c r="K53" t="n">
+        <v>96.66138458251953</v>
       </c>
     </row>
     <row r="54">
@@ -2168,17 +2433,22 @@
       <c r="F54" t="n">
         <v>40.17007780104868</v>
       </c>
-      <c r="G54" t="n">
-        <v>200.9356842041016</v>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H54" t="n">
-        <v>65.72077178955078</v>
+        <v>188.6608276367188</v>
       </c>
       <c r="I54" t="n">
-        <v>92.6646728515625</v>
+        <v>82.69205474853516</v>
       </c>
       <c r="J54" t="n">
-        <v>110.9160919189453</v>
+        <v>170.7070007324219</v>
+      </c>
+      <c r="K54" t="n">
+        <v>103.7849960327148</v>
       </c>
     </row>
     <row r="55">
@@ -2200,17 +2470,22 @@
       <c r="F55" t="n">
         <v>40.31777520333784</v>
       </c>
-      <c r="G55" t="n">
-        <v>205.5767364501953</v>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H55" t="n">
-        <v>61.37221527099609</v>
+        <v>194.5607452392578</v>
       </c>
       <c r="I55" t="n">
-        <v>147.0885009765625</v>
+        <v>79.97234344482422</v>
       </c>
       <c r="J55" t="n">
-        <v>131.3639526367188</v>
+        <v>224.9002075195312</v>
+      </c>
+      <c r="K55" t="n">
+        <v>105.9892807006836</v>
       </c>
     </row>
     <row r="56">
@@ -2232,17 +2507,22 @@
       <c r="F56" t="n">
         <v>38.89328689858721</v>
       </c>
-      <c r="G56" t="n">
-        <v>223.3971099853516</v>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H56" t="n">
-        <v>52.15517044067383</v>
+        <v>205.4769897460938</v>
       </c>
       <c r="I56" t="n">
-        <v>242.7010650634766</v>
+        <v>70.805908203125</v>
       </c>
       <c r="J56" t="n">
-        <v>156.1692199707031</v>
+        <v>296.9824829101562</v>
+      </c>
+      <c r="K56" t="n">
+        <v>117.7498397827148</v>
       </c>
     </row>
     <row r="57">
@@ -2264,17 +2544,22 @@
       <c r="F57" t="n">
         <v>36.03490394546852</v>
       </c>
-      <c r="G57" t="n">
-        <v>259.3802185058594</v>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H57" t="n">
-        <v>43.27840423583984</v>
+        <v>236.4317474365234</v>
       </c>
       <c r="I57" t="n">
-        <v>307.7919006347656</v>
+        <v>63.15375900268555</v>
       </c>
       <c r="J57" t="n">
-        <v>161.8768310546875</v>
+        <v>361.254150390625</v>
+      </c>
+      <c r="K57" t="n">
+        <v>132.1754302978516</v>
       </c>
     </row>
     <row r="58">
@@ -2296,17 +2581,22 @@
       <c r="F58" t="n">
         <v>33.0417017672229</v>
       </c>
-      <c r="G58" t="n">
-        <v>306.3563842773438</v>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H58" t="n">
-        <v>63.26755905151367</v>
+        <v>291.3365478515625</v>
       </c>
       <c r="I58" t="n">
-        <v>353.7831115722656</v>
+        <v>56.04048919677734</v>
       </c>
       <c r="J58" t="n">
-        <v>148.9783630371094</v>
+        <v>364.5771484375</v>
+      </c>
+      <c r="K58" t="n">
+        <v>157.3588714599609</v>
       </c>
     </row>
     <row r="59">
@@ -2328,17 +2618,22 @@
       <c r="F59" t="n">
         <v>43.98768298598323</v>
       </c>
-      <c r="G59" t="n">
-        <v>180.8622131347656</v>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H59" t="n">
-        <v>65.02088165283203</v>
+        <v>181.2554779052734</v>
       </c>
       <c r="I59" t="n">
-        <v>-21.88578796386719</v>
+        <v>63.03110504150391</v>
       </c>
       <c r="J59" t="n">
-        <v>80.85227203369141</v>
+        <v>23.70956611633301</v>
+      </c>
+      <c r="K59" t="n">
+        <v>93.54600524902344</v>
       </c>
     </row>
     <row r="60">
@@ -2360,17 +2655,22 @@
       <c r="F60" t="n">
         <v>45.7006317110727</v>
       </c>
-      <c r="G60" t="n">
-        <v>191.1810150146484</v>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H60" t="n">
-        <v>66.27586364746094</v>
+        <v>190.0792388916016</v>
       </c>
       <c r="I60" t="n">
-        <v>-12.13894557952881</v>
+        <v>69.12972259521484</v>
       </c>
       <c r="J60" t="n">
-        <v>88.91203308105469</v>
+        <v>44.23797988891602</v>
+      </c>
+      <c r="K60" t="n">
+        <v>99.01834106445312</v>
       </c>
     </row>
     <row r="61">
@@ -2392,17 +2692,22 @@
       <c r="F61" t="n">
         <v>46.67965674781412</v>
       </c>
-      <c r="G61" t="n">
-        <v>200.9493255615234</v>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H61" t="n">
-        <v>63.90511322021484</v>
+        <v>192.2933807373047</v>
       </c>
       <c r="I61" t="n">
-        <v>11.0818920135498</v>
+        <v>75.68699645996094</v>
       </c>
       <c r="J61" t="n">
-        <v>97.45040893554688</v>
+        <v>76.81114196777344</v>
+      </c>
+      <c r="K61" t="n">
+        <v>106.8517990112305</v>
       </c>
     </row>
     <row r="62">
@@ -2424,17 +2729,22 @@
       <c r="F62" t="n">
         <v>47.53914448671719</v>
       </c>
-      <c r="G62" t="n">
-        <v>209.0118408203125</v>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H62" t="n">
-        <v>62.10633850097656</v>
+        <v>195.0305786132812</v>
       </c>
       <c r="I62" t="n">
-        <v>34.27471542358398</v>
+        <v>79.21177673339844</v>
       </c>
       <c r="J62" t="n">
-        <v>107.9872817993164</v>
+        <v>108.4671173095703</v>
+      </c>
+      <c r="K62" t="n">
+        <v>106.6386260986328</v>
       </c>
     </row>
     <row r="63">
@@ -2456,17 +2766,22 @@
       <c r="F63" t="n">
         <v>47.07121651777462</v>
       </c>
-      <c r="G63" t="n">
-        <v>212.1057586669922</v>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H63" t="n">
-        <v>59.88686370849609</v>
+        <v>198.7287750244141</v>
       </c>
       <c r="I63" t="n">
-        <v>86.64496612548828</v>
+        <v>86.60434722900391</v>
       </c>
       <c r="J63" t="n">
-        <v>133.6138305664062</v>
+        <v>171.1585235595703</v>
+      </c>
+      <c r="K63" t="n">
+        <v>118.2891540527344</v>
       </c>
     </row>
     <row r="64">
@@ -2488,17 +2803,22 @@
       <c r="F64" t="n">
         <v>45.67156598130153</v>
       </c>
-      <c r="G64" t="n">
-        <v>226.2839813232422</v>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H64" t="n">
-        <v>55.83482360839844</v>
+        <v>209.5943298339844</v>
       </c>
       <c r="I64" t="n">
-        <v>180.1636657714844</v>
+        <v>73.92837524414062</v>
       </c>
       <c r="J64" t="n">
-        <v>161.7836151123047</v>
+        <v>254.9651031494141</v>
+      </c>
+      <c r="K64" t="n">
+        <v>124.2905426025391</v>
       </c>
     </row>
     <row r="65">
@@ -2520,17 +2840,22 @@
       <c r="F65" t="n">
         <v>42.51104340916319</v>
       </c>
-      <c r="G65" t="n">
-        <v>256.0006103515625</v>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H65" t="n">
-        <v>43.48095321655273</v>
+        <v>233.4321136474609</v>
       </c>
       <c r="I65" t="n">
-        <v>258.3962097167969</v>
+        <v>63.89310073852539</v>
       </c>
       <c r="J65" t="n">
-        <v>166.3715362548828</v>
+        <v>324.3525390625</v>
+      </c>
+      <c r="K65" t="n">
+        <v>151.5996551513672</v>
       </c>
     </row>
     <row r="66">
@@ -2552,17 +2877,22 @@
       <c r="F66" t="n">
         <v>54.37577254606605</v>
       </c>
-      <c r="G66" t="n">
-        <v>205.5628814697266</v>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H66" t="n">
-        <v>57.385009765625</v>
+        <v>201.9301605224609</v>
       </c>
       <c r="I66" t="n">
-        <v>-56.69820785522461</v>
+        <v>65.97403717041016</v>
       </c>
       <c r="J66" t="n">
-        <v>97.33146667480469</v>
+        <v>-7.696150779724121</v>
+      </c>
+      <c r="K66" t="n">
+        <v>107.6541519165039</v>
       </c>
     </row>
     <row r="67">
@@ -2584,17 +2914,22 @@
       <c r="F67" t="n">
         <v>55.07062752917076</v>
       </c>
-      <c r="G67" t="n">
-        <v>213.3408966064453</v>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H67" t="n">
-        <v>58.34825897216797</v>
+        <v>202.0468902587891</v>
       </c>
       <c r="I67" t="n">
-        <v>-42.49858474731445</v>
+        <v>75.6116943359375</v>
       </c>
       <c r="J67" t="n">
-        <v>102.0334701538086</v>
+        <v>21.58824920654297</v>
+      </c>
+      <c r="K67" t="n">
+        <v>111.3748397827148</v>
       </c>
     </row>
     <row r="68">
@@ -2616,17 +2951,22 @@
       <c r="F68" t="n">
         <v>54.82432856758766</v>
       </c>
-      <c r="G68" t="n">
-        <v>220.3576507568359</v>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H68" t="n">
-        <v>58.419189453125</v>
+        <v>205.2210540771484</v>
       </c>
       <c r="I68" t="n">
-        <v>-19.79633140563965</v>
+        <v>76.68820190429688</v>
       </c>
       <c r="J68" t="n">
-        <v>110.0754547119141</v>
+        <v>56.33186340332031</v>
+      </c>
+      <c r="K68" t="n">
+        <v>117.2079544067383</v>
       </c>
     </row>
     <row r="69">
@@ -2648,17 +2988,22 @@
       <c r="F69" t="n">
         <v>54.18769809434324</v>
       </c>
-      <c r="G69" t="n">
-        <v>223.1810455322266</v>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H69" t="n">
-        <v>57.34216690063477</v>
+        <v>206.43115234375</v>
       </c>
       <c r="I69" t="n">
-        <v>24.37172508239746</v>
+        <v>84.19795989990234</v>
       </c>
       <c r="J69" t="n">
-        <v>124.734733581543</v>
+        <v>116.4135818481445</v>
+      </c>
+      <c r="K69" t="n">
+        <v>125.5811233520508</v>
       </c>
     </row>
     <row r="70">
@@ -2680,17 +3025,22 @@
       <c r="F70" t="n">
         <v>51.347187815424</v>
       </c>
-      <c r="G70" t="n">
-        <v>228.7630462646484</v>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>FCC</t>
+        </is>
       </c>
       <c r="H70" t="n">
-        <v>55.98562622070312</v>
+        <v>210.4747009277344</v>
       </c>
       <c r="I70" t="n">
-        <v>117.1786575317383</v>
+        <v>77.77152252197266</v>
       </c>
       <c r="J70" t="n">
-        <v>159.501220703125</v>
+        <v>198.7269287109375</v>
+      </c>
+      <c r="K70" t="n">
+        <v>132.9973754882812</v>
       </c>
     </row>
   </sheetData>

</xml_diff>